<commit_message>
replace wrong data by correct data
</commit_message>
<xml_diff>
--- a/final_data/xlsx/results_289_sig.xlsx
+++ b/final_data/xlsx/results_289_sig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelruland/Documents/studium_paderborn/Bachelorarbeit/data_new/association_rules/final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelruland/Documents/studium_paderborn/Bachelorarbeit/BA_thesis/final_data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D891AC65-47B1-454F-9749-046A71169A81}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6590F32D-D328-564F-94CD-5B8135402D86}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results_289_sig" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="80">
   <si>
     <t>antecedent</t>
   </si>
@@ -43,15 +43,24 @@
     <t>(mo_smile;m_gaze_at)</t>
   </si>
   <si>
+    <t>(mother-speech;inf_smile)</t>
+  </si>
+  <si>
     <t>(i_gaze_at;inf_smile)</t>
   </si>
   <si>
     <t>(mother-speech;i_gaze_at;infant_voc)</t>
   </si>
   <si>
+    <t>(mo_smile;inf_smile)</t>
+  </si>
+  <si>
     <t>(mother-speech;m_gaze_at_object)</t>
   </si>
   <si>
+    <t>(infant_voc)</t>
+  </si>
+  <si>
     <t>(i_gaze_at)</t>
   </si>
   <si>
@@ -61,6 +70,9 @@
     <t>(mo_smile)</t>
   </si>
   <si>
+    <t>(m_gaze_at;inf_smile)</t>
+  </si>
+  <si>
     <t>(m_gaze_at;i_gaze_at)</t>
   </si>
   <si>
@@ -70,28 +82,34 @@
     <t>(mother-speech;i_gaze_at)</t>
   </si>
   <si>
+    <t>(m_gaze_at)</t>
+  </si>
+  <si>
     <t>(mo_smile;m_gaze_at;i_gaze_at)</t>
   </si>
   <si>
     <t>(mo_smile;i_gaze_at;inf_smile)</t>
   </si>
   <si>
+    <t>(mother-speech)</t>
+  </si>
+  <si>
     <t>(i_gaze_at;infant_voc)</t>
   </si>
   <si>
     <t>(m_gaze_at;mother-speech)</t>
   </si>
   <si>
+    <t>(inf_smile)</t>
+  </si>
+  <si>
     <t>(m_gaze_away)</t>
   </si>
   <si>
     <t>(m_gaze_at;mother-speech;infant_voc)</t>
   </si>
   <si>
-    <t>(m_gaze_at;inf_smile)</t>
-  </si>
-  <si>
-    <t>(mother-speech;inf_smile)</t>
+    <t>(i_gaze_away)</t>
   </si>
   <si>
     <t>(mo_smile;infant_voc)</t>
@@ -100,63 +118,54 @@
     <t>(mo_smile;i_gaze_at)</t>
   </si>
   <si>
+    <t>(m_gaze_at_object)</t>
+  </si>
+  <si>
     <t>(inf_smile;m_gaze_at_object)</t>
   </si>
   <si>
-    <t>(m_gaze_at)</t>
+    <t>(m_gaze_at;i_gaze_at;inf_smile)</t>
   </si>
   <si>
     <t>(m_gaze_at;i_gaze_at;infant_voc)</t>
   </si>
   <si>
-    <t>(inf_smile)</t>
-  </si>
-  <si>
     <t>(m_gaze_at;mother-speech;inf_smile)</t>
   </si>
   <si>
     <t>(mo_smile;m_gaze_at;inf_smile)</t>
   </si>
   <si>
+    <t>(mo_smile;mother-speech;i_gaze_at)</t>
+  </si>
+  <si>
     <t>(infant_voc;inf_smile)</t>
   </si>
   <si>
     <t>(mo_smile;mother-speech)</t>
   </si>
   <si>
-    <t>(mother-speech)</t>
-  </si>
-  <si>
     <t>(mo_smile;m_gaze_away)</t>
   </si>
   <si>
     <t>(m_gaze_at;mother-speech;i_gaze_at)</t>
   </si>
   <si>
+    <t>(inf_smile;i_gaze_away)</t>
+  </si>
+  <si>
     <t>(m_gaze_at;infant_voc;inf_smile)</t>
   </si>
   <si>
     <t>(mother-speech;m_gaze_away)</t>
   </si>
   <si>
-    <t>(mo_smile;inf_smile)</t>
-  </si>
-  <si>
-    <t>(mo_smile;mother-speech;i_gaze_at)</t>
-  </si>
-  <si>
     <t>(mo_smile;mother-speech;inf_smile)</t>
   </si>
   <si>
     <t>(mother-speech;infant_voc)</t>
   </si>
   <si>
-    <t>(infant_voc)</t>
-  </si>
-  <si>
-    <t>(i_gaze_away)</t>
-  </si>
-  <si>
     <t>(m_gaze_at;i_gaze_at;infant_voc;inf_smile)</t>
   </si>
   <si>
@@ -190,7 +199,7 @@
     <t>(m_gaze_at;infant_voc)</t>
   </si>
   <si>
-    <t>(m_gaze_at;i_gaze_at;inf_smile)</t>
+    <t>(i_gaze_at_object)</t>
   </si>
   <si>
     <t>(mo_smile;i_gaze_away;m_gaze_at_object)</t>
@@ -214,6 +223,9 @@
     <t>(mo_smile;i_gaze_at;m_gaze_at_object)</t>
   </si>
   <si>
+    <t>(mo_smile;i_gaze_away)</t>
+  </si>
+  <si>
     <t>(m_gaze_away;i_gaze_at_object)</t>
   </si>
   <si>
@@ -229,9 +241,6 @@
     <t>(inf_smile;i_gaze_at_object)</t>
   </si>
   <si>
-    <t>(m_gaze_at_object)</t>
-  </si>
-  <si>
     <t>(infant_voc;inf_smile;i_gaze_at_object)</t>
   </si>
   <si>
@@ -251,15 +260,12 @@
   </si>
   <si>
     <t>(mo_smile;m_gaze_at;i_gaze_away)</t>
-  </si>
-  <si>
-    <t>(mo_smile;i_gaze_away)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -798,15 +804,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F279" totalsRowShown="0">
-  <autoFilter ref="A1:F279"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A419ED5C-37C4-D544-9C7A-EBAB4CB219FF}" name="Table1" displayName="Table1" ref="A1:F279" totalsRowShown="0">
+  <autoFilter ref="A1:F279" xr:uid="{EC1DEB2C-5227-2B45-BEB6-0A9C9680DC96}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="antecedent"/>
-    <tableColumn id="2" name="succedent"/>
-    <tableColumn id="3" name="p_con"/>
-    <tableColumn id="4" name="p_occ"/>
-    <tableColumn id="5" name="p_dur"/>
-    <tableColumn id="6" name="null_obs"/>
+    <tableColumn id="1" xr3:uid="{14D3AAC2-7525-4F4E-8A42-DF645C3A93DA}" name="antecedent"/>
+    <tableColumn id="2" xr3:uid="{60A9FDB7-A400-BE41-AE1A-94ACA2A16601}" name="succedent"/>
+    <tableColumn id="3" xr3:uid="{F78AA853-B5D0-DC4A-945E-939903607FFB}" name="p_con"/>
+    <tableColumn id="4" xr3:uid="{5785936C-2114-8645-B518-8D33471B40B4}" name="p_occ"/>
+    <tableColumn id="5" xr3:uid="{66859FE9-A7C1-3745-9CAF-FB172840C75B}" name="p_dur"/>
+    <tableColumn id="6" xr3:uid="{7DDC8C32-4422-1A40-A5D1-788D02F231A7}" name="null_obs"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1108,17 +1114,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F279"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A257" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1146,7 +1152,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1163,10 +1169,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1183,10 +1189,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1203,10 +1209,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>2.7027027027027001E-2</v>
@@ -1223,10 +1229,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>0.30909090909090903</v>
@@ -1243,10 +1249,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>4.7619047619047603E-2</v>
@@ -1266,7 +1272,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1283,10 +1289,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1303,10 +1309,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1323,10 +1329,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>5.7971014492753603E-2</v>
@@ -1343,10 +1349,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1363,10 +1369,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1383,10 +1389,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <v>0.28571428571428498</v>
@@ -1403,10 +1409,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C15">
         <v>5.3571428571428499E-2</v>
@@ -1423,10 +1429,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1443,10 +1449,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>4.3478260869565202E-2</v>
@@ -1463,10 +1469,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>4.8387096774193498E-2</v>
@@ -1483,10 +1489,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C19">
         <v>0.25</v>
@@ -1503,10 +1509,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1523,10 +1529,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1543,10 +1549,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C22">
         <v>0.60869565217391297</v>
@@ -1563,10 +1569,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C23">
         <v>2.6315789473684199E-2</v>
@@ -1583,10 +1589,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1603,10 +1609,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1623,10 +1629,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1643,10 +1649,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1663,10 +1669,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1683,10 +1689,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1703,10 +1709,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1723,10 +1729,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1746,7 +1752,7 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1763,10 +1769,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1783,10 +1789,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1803,10 +1809,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1823,10 +1829,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1843,10 +1849,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1863,10 +1869,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1883,10 +1889,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1903,10 +1909,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1923,10 +1929,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C41">
         <v>0.114285714285714</v>
@@ -1943,10 +1949,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="C42">
         <v>0.02</v>
@@ -1963,10 +1969,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1983,10 +1989,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -2003,10 +2009,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B45" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -2023,10 +2029,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B46" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C46">
         <v>1.4492753623188401E-2</v>
@@ -2043,10 +2049,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C47">
         <v>8.6956521739130405E-2</v>
@@ -2063,10 +2069,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2083,10 +2089,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B49" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2103,10 +2109,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -2123,10 +2129,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -2143,10 +2149,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2163,10 +2169,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B53" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2183,10 +2189,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C54">
         <v>8.3333333333333301E-2</v>
@@ -2203,10 +2209,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B55" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="C55">
         <v>2.4390243902439001E-2</v>
@@ -2223,10 +2229,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B56" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -2243,10 +2249,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B57" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -2263,10 +2269,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B58" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -2283,7 +2289,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B59" t="s">
         <v>15</v>
@@ -2303,10 +2309,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B60" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -2323,10 +2329,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B61" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -2343,10 +2349,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B62" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -2363,10 +2369,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B63" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -2383,10 +2389,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B64" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C64">
         <v>3.6144578313252997E-2</v>
@@ -2403,10 +2409,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -2423,10 +2429,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B66" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C66">
         <v>0.02</v>
@@ -2443,10 +2449,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B67" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -2463,10 +2469,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B68" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -2483,10 +2489,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B69" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -2503,10 +2509,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B70" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -2523,10 +2529,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C71">
         <v>0.46666666666666601</v>
@@ -2543,10 +2549,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B72" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C72">
         <v>0.01</v>
@@ -2563,10 +2569,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B73" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -2583,10 +2589,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B74" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -2603,10 +2609,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B75" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -2623,10 +2629,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B76" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -2643,10 +2649,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B77" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -2663,10 +2669,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B78" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="C78">
         <v>2.94117647058823E-2</v>
@@ -2683,10 +2689,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B79" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -2703,10 +2709,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B80" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -2723,10 +2729,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B81" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -2743,10 +2749,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B82" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -2763,10 +2769,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="B83" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -2783,10 +2789,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B84" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -2803,10 +2809,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B85" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C85">
         <v>0.60465116279069697</v>
@@ -2823,10 +2829,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B86" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2843,10 +2849,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B87" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -2863,10 +2869,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B88" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -2883,10 +2889,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B89" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C89">
         <v>0.34883720930232498</v>
@@ -2903,10 +2909,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B90" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -2923,10 +2929,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B91" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -2943,10 +2949,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B92" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -2963,10 +2969,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B93" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C93">
         <v>0.66666666666666596</v>
@@ -2983,10 +2989,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B94" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -3003,10 +3009,10 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B95" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C95">
         <v>0.5</v>
@@ -3023,10 +3029,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B96" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -3043,10 +3049,10 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B97" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -3063,10 +3069,10 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B98" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -3083,10 +3089,10 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="B99" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -3103,10 +3109,10 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B100" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -3123,10 +3129,10 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B101" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -3143,10 +3149,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B102" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -3163,10 +3169,10 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B103" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -3183,10 +3189,10 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B104" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="C104">
         <v>0.71428571428571397</v>
@@ -3203,10 +3209,10 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B105" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -3223,10 +3229,10 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B106" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -3243,10 +3249,10 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B107" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="C107">
         <v>0.11764705882352899</v>
@@ -3263,10 +3269,10 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B108" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -3283,10 +3289,10 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B109" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -3303,10 +3309,10 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B110" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -3323,10 +3329,10 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B111" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -3343,10 +3349,10 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B112" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -3363,10 +3369,10 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B113" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -3383,10 +3389,10 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B114" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -3403,10 +3409,10 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B115" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -3423,10 +3429,10 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B116" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -3443,10 +3449,10 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B117" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -3463,10 +3469,10 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B118" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -3483,10 +3489,10 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B119" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C119">
         <v>0</v>
@@ -3503,10 +3509,10 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B120" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -3523,10 +3529,10 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B121" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -3543,10 +3549,10 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B122" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -3563,10 +3569,10 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B123" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -3583,10 +3589,10 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B124" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C124">
         <v>0.98</v>
@@ -3603,10 +3609,10 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B125" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -3623,10 +3629,10 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B126" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C126">
         <v>1.7543859649122799E-2</v>
@@ -3643,10 +3649,10 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B127" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C127">
         <v>0</v>
@@ -3663,10 +3669,10 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B128" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C128">
         <v>1.42857142857142E-2</v>
@@ -3683,10 +3689,10 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B129" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="C129">
         <v>0</v>
@@ -3703,10 +3709,10 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B130" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -3723,10 +3729,10 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B131" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -3743,10 +3749,10 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B132" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="C132">
         <v>4.7619047619047603E-2</v>
@@ -3763,10 +3769,10 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B133" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -3783,10 +3789,10 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B134" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -3803,10 +3809,10 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B135" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C135">
         <v>0.05</v>
@@ -3823,10 +3829,10 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B136" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C136">
         <v>2.3809523809523801E-2</v>
@@ -3843,10 +3849,10 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B137" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -3863,10 +3869,10 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B138" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -3883,10 +3889,10 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B139" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -3903,10 +3909,10 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B140" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -3923,10 +3929,10 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B141" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C141">
         <v>0</v>
@@ -3943,10 +3949,10 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B142" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C142">
         <v>0</v>
@@ -3963,10 +3969,10 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B143" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C143">
         <v>0</v>
@@ -3983,10 +3989,10 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B144" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="C144">
         <v>0</v>
@@ -4003,10 +4009,10 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B145" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="C145">
         <v>0</v>
@@ -4023,10 +4029,10 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B146" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C146">
         <v>0</v>
@@ -4043,10 +4049,10 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B147" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="C147">
         <v>0</v>
@@ -4063,10 +4069,10 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B148" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -4083,10 +4089,10 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B149" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C149">
         <v>0.42857142857142799</v>
@@ -4103,10 +4109,10 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B150" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -4123,10 +4129,10 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B151" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C151">
         <v>0</v>
@@ -4143,10 +4149,10 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B152" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -4163,10 +4169,10 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B153" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C153">
         <v>0</v>
@@ -4183,10 +4189,10 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B154" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="C154">
         <v>5.8823529411764698E-2</v>
@@ -4203,10 +4209,10 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B155" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -4223,10 +4229,10 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B156" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -4243,10 +4249,10 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B157" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -4263,10 +4269,10 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B158" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -4283,10 +4289,10 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B159" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -4303,10 +4309,10 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B160" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C160">
         <v>0</v>
@@ -4323,10 +4329,10 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B161" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C161">
         <v>0.14285714285714199</v>
@@ -4343,10 +4349,10 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B162" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="C162">
         <v>1.8867924528301799E-2</v>
@@ -4363,10 +4369,10 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B163" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -4383,10 +4389,10 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B164" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="C164">
         <v>0.875</v>
@@ -4403,10 +4409,10 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B165" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="C165">
         <v>2.3809523809523801E-2</v>
@@ -4423,10 +4429,10 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B166" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C166">
         <v>0</v>
@@ -4443,10 +4449,10 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B167" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="C167">
         <v>0</v>
@@ -4463,10 +4469,10 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B168" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="C168">
         <v>3.3333333333333298E-2</v>
@@ -4483,10 +4489,10 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B169" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="C169">
         <v>0</v>
@@ -4503,10 +4509,10 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B170" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="C170">
         <v>0</v>
@@ -4523,10 +4529,10 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B171" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C171">
         <v>0</v>
@@ -4546,7 +4552,7 @@
         <v>6</v>
       </c>
       <c r="B172" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C172">
         <v>0.5</v>
@@ -4563,10 +4569,10 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B173" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C173">
         <v>4.8780487804878002E-2</v>
@@ -4583,10 +4589,10 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B174" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C174">
         <v>0.16</v>
@@ -4603,10 +4609,10 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B175" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C175">
         <v>0.02</v>
@@ -4623,10 +4629,10 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B176" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C176">
         <v>0</v>
@@ -4643,10 +4649,10 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B177" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C177">
         <v>0</v>
@@ -4663,10 +4669,10 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B178" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C178">
         <v>0</v>
@@ -4686,7 +4692,7 @@
         <v>6</v>
       </c>
       <c r="B179" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C179">
         <v>0</v>
@@ -4703,10 +4709,10 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B180" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C180">
         <v>1.2820512820512799E-2</v>
@@ -4723,10 +4729,10 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="B181" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="C181">
         <v>1.38888888888888E-2</v>
@@ -4743,10 +4749,10 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B182" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C182">
         <v>0</v>
@@ -4763,10 +4769,10 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B183" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C183">
         <v>9.0909090909090898E-2</v>
@@ -4783,10 +4789,10 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B184" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C184">
         <v>0</v>
@@ -4803,10 +4809,10 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B185" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C185">
         <v>1</v>
@@ -4823,10 +4829,10 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B186" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="C186">
         <v>0.86666666666666603</v>
@@ -4843,10 +4849,10 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B187" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="C187">
         <v>0</v>
@@ -4863,10 +4869,10 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B188" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C188">
         <v>0.339622641509433</v>
@@ -4883,10 +4889,10 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B189" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C189">
         <v>0.01</v>
@@ -4903,10 +4909,10 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B190" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C190">
         <v>0</v>
@@ -4923,10 +4929,10 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B191" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C191">
         <v>1.47058823529411E-2</v>
@@ -4943,10 +4949,10 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B192" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="C192">
         <v>0</v>
@@ -4966,7 +4972,7 @@
         <v>6</v>
       </c>
       <c r="B193" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C193">
         <v>0</v>
@@ -4983,10 +4989,10 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B194" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="C194">
         <v>0</v>
@@ -5003,10 +5009,10 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B195" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="C195">
         <v>0</v>
@@ -5023,10 +5029,10 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="B196" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C196">
         <v>1.35135135135135E-2</v>
@@ -5043,10 +5049,10 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B197" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C197">
         <v>0</v>
@@ -5063,10 +5069,10 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B198" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C198">
         <v>0</v>
@@ -5083,10 +5089,10 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B199" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="C199">
         <v>0</v>
@@ -5103,10 +5109,10 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B200" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C200">
         <v>0</v>
@@ -5123,10 +5129,10 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B201" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C201">
         <v>0</v>
@@ -5143,10 +5149,10 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B202" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="C202">
         <v>0</v>
@@ -5163,10 +5169,10 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B203" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C203">
         <v>0</v>
@@ -5183,10 +5189,10 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B204" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C204">
         <v>0</v>
@@ -5203,10 +5209,10 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B205" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C205">
         <v>0</v>
@@ -5223,10 +5229,10 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B206" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C206">
         <v>0</v>
@@ -5243,10 +5249,10 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B207" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C207">
         <v>1</v>
@@ -5263,10 +5269,10 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B208" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C208">
         <v>3.7735849056603703E-2</v>
@@ -5283,10 +5289,10 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B209" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="C209">
         <v>0</v>
@@ -5303,10 +5309,10 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B210" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="C210">
         <v>0.17647058823529399</v>
@@ -5323,10 +5329,10 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B211" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C211">
         <v>0</v>
@@ -5343,10 +5349,10 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B212" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C212">
         <v>0</v>
@@ -5363,10 +5369,10 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B213" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="C213">
         <v>0</v>
@@ -5383,10 +5389,10 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B214" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="C214">
         <v>0.11111111111111099</v>
@@ -5403,10 +5409,10 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B215" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="C215">
         <v>0</v>
@@ -5423,10 +5429,10 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="B216" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C216">
         <v>0.1</v>
@@ -5443,10 +5449,10 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B217" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C217">
         <v>0</v>
@@ -5463,10 +5469,10 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B218" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="C218">
         <v>2.3809523809523801E-2</v>
@@ -5483,10 +5489,10 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B219" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C219">
         <v>0</v>
@@ -5503,10 +5509,10 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B220" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="C220">
         <v>0</v>
@@ -5523,10 +5529,10 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B221" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C221">
         <v>0</v>
@@ -5543,10 +5549,10 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B222" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C222">
         <v>0</v>
@@ -5563,10 +5569,10 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B223" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C223">
         <v>0</v>
@@ -5583,10 +5589,10 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B224" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C224">
         <v>0</v>
@@ -5603,10 +5609,10 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B225" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C225">
         <v>0</v>
@@ -5623,10 +5629,10 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B226" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C226">
         <v>0</v>
@@ -5643,10 +5649,10 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B227" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="C227">
         <v>0</v>
@@ -5663,10 +5669,10 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B228" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C228">
         <v>0</v>
@@ -5683,10 +5689,10 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B229" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="C229">
         <v>0.16666666666666599</v>
@@ -5703,10 +5709,10 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B230" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="C230">
         <v>0</v>
@@ -5723,10 +5729,10 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B231" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C231">
         <v>0</v>
@@ -5743,10 +5749,10 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B232" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="C232">
         <v>0</v>
@@ -5763,10 +5769,10 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B233" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C233">
         <v>0</v>
@@ -5783,10 +5789,10 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B234" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C234">
         <v>0</v>
@@ -5803,10 +5809,10 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B235" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="C235">
         <v>0</v>
@@ -5823,7 +5829,7 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B236" t="s">
         <v>25</v>
@@ -5843,10 +5849,10 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B237" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C237">
         <v>0</v>
@@ -5863,10 +5869,10 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B238" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C238">
         <v>0</v>
@@ -5883,10 +5889,10 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B239" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C239">
         <v>0.125</v>
@@ -5903,10 +5909,10 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B240" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C240">
         <v>0</v>
@@ -5923,10 +5929,10 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B241" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C241">
         <v>0</v>
@@ -5943,10 +5949,10 @@
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B242" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C242">
         <v>0</v>
@@ -5963,10 +5969,10 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B243" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C243">
         <v>0</v>
@@ -5983,10 +5989,10 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B244" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="C244">
         <v>0</v>
@@ -6003,10 +6009,10 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B245" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C245">
         <v>0</v>
@@ -6023,10 +6029,10 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B246" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C246">
         <v>0.120481927710843</v>
@@ -6043,10 +6049,10 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B247" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="C247">
         <v>0</v>
@@ -6063,7 +6069,7 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B248" t="s">
         <v>10</v>
@@ -6083,10 +6089,10 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B249" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="C249">
         <v>0</v>
@@ -6103,10 +6109,10 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B250" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C250">
         <v>0</v>
@@ -6123,10 +6129,10 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B251" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C251">
         <v>0</v>
@@ -6143,10 +6149,10 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B252" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="C252">
         <v>0</v>
@@ -6163,10 +6169,10 @@
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B253" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C253">
         <v>0</v>
@@ -6183,10 +6189,10 @@
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B254" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="C254">
         <v>0</v>
@@ -6203,10 +6209,10 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B255" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C255">
         <v>0.17391304347826</v>
@@ -6223,10 +6229,10 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B256" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C256">
         <v>0</v>
@@ -6243,10 +6249,10 @@
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B257" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C257">
         <v>0</v>
@@ -6263,10 +6269,10 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B258" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="C258">
         <v>4.6875E-2</v>
@@ -6283,10 +6289,10 @@
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B259" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="C259">
         <v>0.125</v>
@@ -6303,10 +6309,10 @@
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B260" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C260">
         <v>0</v>
@@ -6323,10 +6329,10 @@
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B261" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C261">
         <v>0.04</v>
@@ -6343,10 +6349,10 @@
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B262" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C262">
         <v>0</v>
@@ -6363,10 +6369,10 @@
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B263" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C263">
         <v>0</v>
@@ -6383,10 +6389,10 @@
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B264" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C264">
         <v>2.6315789473684199E-2</v>
@@ -6403,10 +6409,10 @@
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B265" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C265">
         <v>0</v>
@@ -6423,10 +6429,10 @@
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B266" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C266">
         <v>0</v>
@@ -6446,7 +6452,7 @@
         <v>6</v>
       </c>
       <c r="B267" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C267">
         <v>0.2</v>
@@ -6463,10 +6469,10 @@
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B268" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C268">
         <v>0</v>
@@ -6483,10 +6489,10 @@
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B269" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C269">
         <v>0</v>
@@ -6503,10 +6509,10 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B270" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C270">
         <v>0</v>
@@ -6523,10 +6529,10 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B271" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C271">
         <v>0</v>
@@ -6543,10 +6549,10 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B272" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C272">
         <v>0</v>
@@ -6563,10 +6569,10 @@
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B273" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="C273">
         <v>0</v>
@@ -6583,10 +6589,10 @@
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B274" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C274">
         <v>0</v>
@@ -6603,10 +6609,10 @@
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B275" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C275">
         <v>0.58333333333333304</v>
@@ -6623,10 +6629,10 @@
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B276" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C276">
         <v>0</v>
@@ -6643,10 +6649,10 @@
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B277" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C277">
         <v>0</v>
@@ -6663,10 +6669,10 @@
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B278" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C278">
         <v>0.48648648648648601</v>
@@ -6683,7 +6689,7 @@
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B279" t="s">
         <v>29</v>

</xml_diff>